<commit_message>
gw: update guinea bissau forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Guinnée Bissau/gw_lf_pretas_1_sites_202206.xlsx
+++ b/LF/PreTAS/Guinnée Bissau/gw_lf_pretas_1_sites_202206.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="95">
   <si>
     <t>type</t>
   </si>
@@ -254,6 +254,9 @@
     <t>Paunca</t>
   </si>
   <si>
+    <t>Pitche</t>
+  </si>
+  <si>
     <t>Beli-Pataqui</t>
   </si>
   <si>
@@ -278,16 +281,22 @@
     <t>allow_choice_duplicates</t>
   </si>
   <si>
-    <t>(Jun 2022) 7. Pre TAS1 FL - Formulário do site V2.1</t>
-  </si>
-  <si>
-    <t>gw_lf_pretas_1_sites_202206_v2_1</t>
+    <t>(Aug 2022) 7. Pre TAS FL - Formulário do site (Phase 2)</t>
+  </si>
+  <si>
+    <t>gw_lf_pretas_1_sites_202208_phase2</t>
   </si>
   <si>
     <t>Portuguese</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Region</t>
     </r>
     <r>
@@ -301,6 +310,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Health area</t>
     </r>
     <r>
@@ -330,9 +345,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="29">
@@ -379,8 +394,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,8 +418,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,6 +435,66 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -424,45 +508,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,23 +517,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -497,13 +542,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -513,30 +551,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -562,31 +577,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,151 +643,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,24 +861,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -875,32 +872,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -928,153 +899,197 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1890,12 +1905,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18:F21"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -2055,26 +2070,26 @@
       <c r="E11" s="14"/>
     </row>
     <row r="12" s="8" customFormat="1" spans="1:5">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="A12" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="E12" s="14"/>
     </row>
     <row r="13" s="8" customFormat="1" spans="1:5">
-      <c r="A13" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17" t="s">
-        <v>75</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" s="8" customFormat="1" spans="1:5">
       <c r="A14" s="14" t="s">
@@ -2088,7 +2103,7 @@
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" s="8" customFormat="1" spans="1:5">
@@ -2103,7 +2118,7 @@
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" s="8" customFormat="1" spans="1:5">
@@ -2111,53 +2126,55 @@
         <v>66</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" s="8" customFormat="1" spans="1:5">
+      <c r="A17" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18">
-        <v>1001</v>
-      </c>
-      <c r="C18">
-        <v>1001</v>
-      </c>
-      <c r="F18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19">
-        <v>1002</v>
-      </c>
-      <c r="C19">
-        <v>1002</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="C17" s="17" t="s">
         <v>74</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" s="8" customFormat="1" spans="1:5">
+      <c r="A18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B20">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C20">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="F20" t="s">
         <v>79</v>
@@ -2165,15 +2182,57 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21">
+        <v>1002</v>
+      </c>
+      <c r="C21">
+        <v>1002</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22">
+        <v>1003</v>
+      </c>
+      <c r="C22">
+        <v>1003</v>
+      </c>
+      <c r="F22" t="s">
         <v>80</v>
       </c>
-      <c r="B21">
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23">
         <v>1004</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>1004</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24">
+        <v>1005</v>
+      </c>
+      <c r="C24">
+        <v>1005</v>
+      </c>
+      <c r="F24" s="15" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2192,39 +2251,41 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="44.1259259259259" customWidth="1"/>
-    <col min="2" max="2" width="31.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="48.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="35.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="15.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="21.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2261,32 +2322,32 @@
   <sheetData>
     <row r="1" ht="15" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E1" s="4"/>
       <c r="G1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -2297,10 +2358,10 @@
         <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2">
         <v>1001</v>
@@ -2318,7 +2379,7 @@
         <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2332,7 +2393,7 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E3">
         <v>1002</v>
@@ -2350,7 +2411,7 @@
         <v>73</v>
       </c>
       <c r="M3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2361,10 +2422,10 @@
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4">
         <v>1003</v>
@@ -2379,7 +2440,7 @@
         <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2390,10 +2451,10 @@
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E5">
         <v>1004</v>

</xml_diff>